<commit_message>
Some WIP made on the auto-calibration. 1 MHz almost working, 3 MHz has problems on hardware with 10 pre-series PCBs. Pending on receiving prototype PCB from Rös's for checking changes
</commit_message>
<xml_diff>
--- a/20171212 - taules definitives vrms.xlsx
+++ b/20171212 - taules definitives vrms.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="36" windowWidth="17124" windowHeight="6096" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="96" windowWidth="17124" windowHeight="6036" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>%</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>3MHZ Facial</t>
+  </si>
+  <si>
+    <t>Index</t>
   </si>
 </sst>
 </file>
@@ -410,7 +413,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection sqref="A1:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -755,609 +758,695 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F22"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="6"/>
-    <col min="3" max="3" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="0" style="6" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="2" width="11.5546875" style="6"/>
+    <col min="4" max="4" width="0" style="6" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="0" style="6" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="0" style="6" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="7"/>
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
+    <row r="2" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
         <v>0</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="7">
         <v>0</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5">
+      <c r="C2" s="5">
         <v>0</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5">
+      <c r="D2" s="5"/>
+      <c r="E2" s="5">
         <v>0</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5">
+      <c r="F2" s="5"/>
+      <c r="G2" s="5">
         <v>0</v>
       </c>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="7">
-        <f>A2+5</f>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="8"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
+        <f>B2+5</f>
         <v>5</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C3" s="1">
         <v>74.400000000000006</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1">
+      <c r="D3" s="1"/>
+      <c r="E3" s="1">
         <v>43.3</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1">
+      <c r="F3" s="1"/>
+      <c r="G3" s="1">
         <v>41.8</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1">
         <v>24.7</v>
       </c>
-      <c r="I3" s="8"/>
-    </row>
-    <row r="4" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
-        <f>A3+5</f>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <f t="shared" ref="A4:A22" si="0">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="7">
+        <f>B3+5</f>
         <v>10</v>
       </c>
-      <c r="B4" s="1">
-        <f>B3+$C$4</f>
+      <c r="C4" s="1">
+        <f>C3+$D$4</f>
         <v>75.75</v>
       </c>
-      <c r="C4" s="1">
-        <f>((B7-B3)/(($A$7-$A$3)/5))</f>
+      <c r="D4" s="1">
+        <f>((C7-C3)/(($B$7-$B$3)/5))</f>
         <v>1.3499999999999979</v>
       </c>
-      <c r="D4" s="1">
-        <f>D3+$E$4</f>
+      <c r="E4" s="1">
+        <f>E3+$F$4</f>
         <v>47.424999999999997</v>
       </c>
-      <c r="E4" s="1">
-        <f>((D7-D3)/(($A$7-$A$3)/5))</f>
+      <c r="F4" s="1">
+        <f>((E7-E3)/(($B$7-$B$3)/5))</f>
         <v>4.125</v>
       </c>
-      <c r="F4" s="1">
-        <f>F3+$G$4</f>
+      <c r="G4" s="1">
+        <f>G3+$H$4</f>
         <v>44.699999999999996</v>
       </c>
-      <c r="G4" s="1">
-        <f>((F7-F3)/(($A$7-$A$3)/5))</f>
+      <c r="H4" s="1">
+        <f>((G7-G3)/(($B$7-$B$3)/5))</f>
         <v>2.9000000000000004</v>
       </c>
-      <c r="H4" s="1">
-        <f>H3+$I$4</f>
+      <c r="I4" s="1">
+        <f>I3+$J$4</f>
         <v>27.474999999999998</v>
       </c>
-      <c r="I4" s="1">
-        <f>((H7-H3)/(($A$7-$A$3)/5))</f>
+      <c r="J4" s="1">
+        <f>((I7-I3)/(($B$7-$B$3)/5))</f>
         <v>2.7749999999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
-        <f t="shared" ref="A5:A22" si="0">A4+5</f>
+    <row r="5" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="7">
+        <f t="shared" ref="B5:B22" si="1">B4+5</f>
         <v>15</v>
       </c>
-      <c r="B5" s="1">
-        <f>B4+$C$4</f>
+      <c r="C5" s="1">
+        <f>C4+$D$4</f>
         <v>77.099999999999994</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1">
-        <f t="shared" ref="D5:D6" si="1">D4+$E$4</f>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1">
+        <f t="shared" ref="E5:E6" si="2">E4+$F$4</f>
         <v>51.55</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1">
-        <f t="shared" ref="F5:F6" si="2">F4+$G$4</f>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1">
+        <f t="shared" ref="G5:G6" si="3">G4+$H$4</f>
         <v>47.599999999999994</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1">
-        <f t="shared" ref="H5:H11" si="3">H4+$I$4</f>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1">
+        <f t="shared" ref="I5:I6" si="4">I4+$J$4</f>
         <v>30.249999999999996</v>
       </c>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
-        <f t="shared" si="0"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="7">
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B6" s="1">
-        <f>B5+$C$4</f>
+      <c r="C6" s="1">
+        <f>C5+$D$4</f>
         <v>78.449999999999989</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1">
-        <f t="shared" si="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1">
+        <f t="shared" si="2"/>
         <v>55.674999999999997</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1">
-        <f t="shared" si="2"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1">
+        <f t="shared" si="3"/>
         <v>50.499999999999993</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1">
-        <f t="shared" si="3"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1">
+        <f t="shared" si="4"/>
         <v>33.024999999999999</v>
       </c>
-      <c r="I6" s="8"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
-        <f t="shared" si="0"/>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="7">
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="B7" s="1">
+      <c r="C7" s="1">
         <v>79.8</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1">
         <v>59.8</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1">
         <v>53.4</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1">
+      <c r="H7" s="1"/>
+      <c r="I7" s="1">
         <v>35.799999999999997</v>
       </c>
-      <c r="I7" s="8"/>
-    </row>
-    <row r="8" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
-        <f t="shared" si="0"/>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="7">
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B8" s="1">
-        <f>B7+$C$8</f>
+      <c r="C8" s="1">
+        <f>C7+$D$8</f>
         <v>80.2</v>
       </c>
-      <c r="C8" s="1">
-        <f>((B12-B7)/(($A$12-$A$7)/5))</f>
+      <c r="D8" s="1">
+        <f>((C12-C7)/(($B$12-$B$7)/5))</f>
         <v>0.4</v>
       </c>
-      <c r="D8" s="1">
-        <f>D7+$E$8</f>
+      <c r="E8" s="1">
+        <f>E7+$F$8</f>
         <v>63.199999999999996</v>
       </c>
-      <c r="E8" s="1">
-        <f>((D12-D7)/(($A$12-$A$7)/5))</f>
+      <c r="F8" s="1">
+        <f>((E12-E7)/(($B$12-$B$7)/5))</f>
         <v>3.4</v>
       </c>
-      <c r="F8" s="1">
-        <f>F7+$G$8</f>
+      <c r="G8" s="1">
+        <f>G7+$H$8</f>
         <v>55.28</v>
       </c>
-      <c r="G8" s="1">
-        <f>((F12-F7)/(($A$12-$A$7)/5))</f>
+      <c r="H8" s="1">
+        <f>((G12-G7)/(($B$12-$B$7)/5))</f>
         <v>1.8799999999999997</v>
       </c>
-      <c r="H8" s="1">
-        <f>H7+$I$8</f>
+      <c r="I8" s="1">
+        <f>I7+$J$8</f>
         <v>39.4</v>
       </c>
-      <c r="I8" s="1">
-        <f>((H12-H7)/(($A$12-$A$7)/5))</f>
+      <c r="J8" s="1">
+        <f>((I12-I7)/(($B$12-$B$7)/5))</f>
         <v>3.6</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
-        <f t="shared" si="0"/>
+    <row r="9" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="7">
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="B9" s="1">
-        <f t="shared" ref="B9:B11" si="4">B8+$C$8</f>
+      <c r="C9" s="1">
+        <f t="shared" ref="C9:C11" si="5">C8+$D$8</f>
         <v>80.600000000000009</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1">
-        <f t="shared" ref="D9:D11" si="5">D8+$E$8</f>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1">
+        <f t="shared" ref="E9:E11" si="6">E8+$F$8</f>
         <v>66.599999999999994</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1">
-        <f t="shared" ref="F9:F11" si="6">F8+$G$8</f>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1">
+        <f t="shared" ref="G9:G11" si="7">G8+$H$8</f>
         <v>57.160000000000004</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1">
-        <f t="shared" ref="H9:H11" si="7">H8+$I$8</f>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1">
+        <f t="shared" ref="I9:I11" si="8">I8+$J$8</f>
         <v>43</v>
       </c>
-      <c r="I9" s="8"/>
-    </row>
-    <row r="10" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
-        <f t="shared" si="0"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="7">
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="B10" s="1">
-        <f t="shared" si="4"/>
+      <c r="C10" s="1">
+        <f t="shared" si="5"/>
         <v>81.000000000000014</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1">
+        <f t="shared" si="6"/>
+        <v>70</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1">
+        <f t="shared" si="7"/>
+        <v>59.040000000000006</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1">
+        <f t="shared" si="8"/>
+        <v>46.6</v>
+      </c>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="7">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="C11" s="1">
         <f t="shared" si="5"/>
+        <v>81.40000000000002</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1">
+        <f t="shared" si="6"/>
+        <v>73.400000000000006</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1">
+        <f t="shared" si="7"/>
+        <v>60.920000000000009</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1">
+        <f t="shared" si="8"/>
+        <v>50.2</v>
+      </c>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="7">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="C12" s="1">
+        <v>81.8</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1">
+        <v>76.8</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1">
+        <v>62.8</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1">
+        <v>53.8</v>
+      </c>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="7">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="C13" s="1">
+        <f>C12+$D$13</f>
+        <v>82.12</v>
+      </c>
+      <c r="D13" s="1">
+        <f>((C17-C12)/(($B$17-$B$12)/5))</f>
+        <v>0.32000000000000173</v>
+      </c>
+      <c r="E13" s="1">
+        <f>E12+$F$13</f>
+        <v>78.02</v>
+      </c>
+      <c r="F13" s="1">
+        <f>((E17-E12)/(($B$17-$B$12)/5))</f>
+        <v>1.2200000000000017</v>
+      </c>
+      <c r="G13" s="1">
+        <f>G12+$H$13</f>
+        <v>64.12</v>
+      </c>
+      <c r="H13" s="1">
+        <f>((G17-G12)/(($B$17-$B$12)/5))</f>
+        <v>1.3200000000000016</v>
+      </c>
+      <c r="I13" s="1">
+        <f>I12+$J$13</f>
+        <v>56.72</v>
+      </c>
+      <c r="J13" s="1">
+        <f>((I17-I12)/(($B$17-$B$12)/5))</f>
+        <v>2.9200000000000017</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="7">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" ref="C14:C16" si="9">C13+$D$13</f>
+        <v>82.440000000000012</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1">
+        <f t="shared" ref="E14:E16" si="10">E13+$F$13</f>
+        <v>79.239999999999995</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1">
+        <f t="shared" ref="G14:G16" si="11">G13+$H$13</f>
+        <v>65.440000000000012</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1">
+        <f t="shared" ref="I14:I16" si="12">I13+$J$13</f>
+        <v>59.64</v>
+      </c>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="7">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="9"/>
+        <v>82.760000000000019</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1">
+        <f t="shared" si="10"/>
+        <v>80.459999999999994</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1">
+        <f t="shared" si="11"/>
+        <v>66.760000000000019</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1">
+        <f t="shared" si="12"/>
+        <v>62.56</v>
+      </c>
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="7">
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1">
-        <f t="shared" si="6"/>
-        <v>59.040000000000006</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1">
-        <f t="shared" si="7"/>
-        <v>46.6</v>
-      </c>
-      <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="B11" s="1">
-        <f t="shared" si="4"/>
-        <v>81.40000000000002</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1">
-        <f t="shared" si="5"/>
-        <v>73.400000000000006</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1">
-        <f t="shared" si="6"/>
-        <v>60.920000000000009</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1">
-        <f t="shared" si="7"/>
-        <v>50.2</v>
-      </c>
-      <c r="I11" s="8"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="7">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="B12" s="1">
-        <v>81.8</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1">
-        <v>76.8</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1">
-        <v>62.8</v>
-      </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1">
-        <v>53.8</v>
-      </c>
-      <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="B13" s="1">
-        <f>B12+$C$13</f>
-        <v>82.12</v>
-      </c>
-      <c r="C13" s="1">
-        <f>((B17-B12)/(($A$17-$A$12)/5))</f>
-        <v>0.32000000000000173</v>
-      </c>
-      <c r="D13" s="1">
-        <f>D12+$E$13</f>
-        <v>78.02</v>
-      </c>
-      <c r="E13" s="1">
-        <f>((D17-D12)/(($A$17-$A$12)/5))</f>
-        <v>1.2200000000000017</v>
-      </c>
-      <c r="F13" s="1">
-        <f>F12+$G$13</f>
-        <v>64.12</v>
-      </c>
-      <c r="G13" s="1">
-        <f>((F17-F12)/(($A$17-$A$12)/5))</f>
-        <v>1.3200000000000016</v>
-      </c>
-      <c r="H13" s="1">
-        <f>H12+$I$13</f>
-        <v>56.72</v>
-      </c>
-      <c r="I13" s="1">
-        <f>((H17-H12)/(($A$17-$A$12)/5))</f>
-        <v>2.9200000000000017</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="B14" s="1">
-        <f t="shared" ref="B14:B19" si="8">B13+$C$13</f>
-        <v>82.440000000000012</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1">
-        <f t="shared" ref="D14:D16" si="9">D13+$E$13</f>
-        <v>79.239999999999995</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1">
-        <f t="shared" ref="F14:F16" si="10">F13+$G$13</f>
-        <v>65.440000000000012</v>
-      </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1">
-        <f t="shared" ref="H14:H16" si="11">H13+$I$13</f>
-        <v>59.64</v>
-      </c>
-      <c r="I14" s="8"/>
-    </row>
-    <row r="15" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="B15" s="1">
-        <f t="shared" si="8"/>
-        <v>82.760000000000019</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1">
+      <c r="C16" s="1">
         <f t="shared" si="9"/>
-        <v>80.459999999999994</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1">
+        <v>83.080000000000027</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1">
         <f t="shared" si="10"/>
-        <v>66.760000000000019</v>
-      </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1">
+        <v>81.679999999999993</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1">
         <f t="shared" si="11"/>
-        <v>62.56</v>
-      </c>
-      <c r="I15" s="8"/>
-    </row>
-    <row r="16" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="B16" s="1">
-        <f t="shared" si="8"/>
-        <v>83.080000000000027</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1">
-        <f t="shared" si="9"/>
-        <v>81.679999999999993</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1">
-        <f t="shared" si="10"/>
         <v>68.080000000000027</v>
       </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1">
-        <f t="shared" si="11"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1">
+        <f t="shared" si="12"/>
         <v>65.48</v>
       </c>
-      <c r="I16" s="8"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="7">
-        <f t="shared" si="0"/>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="7">
+        <f t="shared" si="1"/>
         <v>75</v>
       </c>
-      <c r="B17" s="1">
+      <c r="C17" s="1">
         <v>83.4</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1">
         <v>82.9</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1">
+      <c r="F17" s="1"/>
+      <c r="G17" s="1">
         <v>69.400000000000006</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1">
+      <c r="H17" s="1"/>
+      <c r="I17" s="1">
         <v>68.400000000000006</v>
       </c>
-      <c r="I17" s="8"/>
-    </row>
-    <row r="18" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="7">
-        <f t="shared" si="0"/>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="7">
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="B18" s="1">
-        <f>B17+$C$18</f>
+      <c r="C18" s="1">
+        <f>C17+$D$18</f>
         <v>83.76</v>
       </c>
-      <c r="C18" s="1">
-        <f>((B22-B17)/(($A$22-$A$17)/5))</f>
+      <c r="D18" s="1">
+        <f>((C22-C17)/(($B$22-$B$17)/5))</f>
         <v>0.35999999999999943</v>
       </c>
-      <c r="D18" s="1">
-        <f>D17+$E$18</f>
+      <c r="E18" s="1">
+        <f>E17+$F$18</f>
         <v>83.300000000000011</v>
       </c>
-      <c r="E18" s="1">
-        <f>((D22-D17)/(($A$22-$A$17)/5))</f>
+      <c r="F18" s="1">
+        <f>((E22-E17)/(($B$22-$B$17)/5))</f>
         <v>0.4</v>
       </c>
-      <c r="F18" s="1">
-        <f>F17+$G$18</f>
+      <c r="G18" s="1">
+        <f>G17+$H$18</f>
         <v>70.58</v>
       </c>
-      <c r="G18" s="1">
-        <f>((F22-F17)/(($A$22-$A$17)/5))</f>
+      <c r="H18" s="1">
+        <f>((G22-G17)/(($B$22-$B$17)/5))</f>
         <v>1.1799999999999984</v>
       </c>
-      <c r="H18" s="1">
-        <f>H17+$I$18</f>
+      <c r="I18" s="1">
+        <f>I17+$J$18</f>
         <v>70.94</v>
       </c>
-      <c r="I18" s="1">
-        <f>((H22-H17)/(($A$22-$A$17)/5))</f>
+      <c r="J18" s="1">
+        <f>((I22-I17)/(($B$22-$B$17)/5))</f>
         <v>2.5399999999999978</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7">
-        <f t="shared" si="0"/>
+    <row r="19" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B19" s="7">
+        <f t="shared" si="1"/>
         <v>85</v>
       </c>
-      <c r="B19" s="1">
-        <f t="shared" ref="B19:D21" si="12">B18+$C$18</f>
+      <c r="C19" s="1">
+        <f t="shared" ref="C19:C21" si="13">C18+$D$18</f>
         <v>84.12</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1">
-        <f t="shared" ref="D19:D21" si="13">D18+$E$18</f>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1">
+        <f t="shared" ref="E19:E21" si="14">E18+$F$18</f>
         <v>83.700000000000017</v>
       </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1">
-        <f t="shared" ref="F19:F21" si="14">F18+$G$18</f>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1">
+        <f t="shared" ref="G19:G21" si="15">G18+$H$18</f>
         <v>71.759999999999991</v>
       </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1">
-        <f t="shared" ref="H19:H21" si="15">H18+$I$18</f>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1">
+        <f t="shared" ref="I19:I21" si="16">I18+$J$18</f>
         <v>73.47999999999999</v>
       </c>
-      <c r="I19" s="8"/>
-    </row>
-    <row r="20" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="7">
-        <f t="shared" si="0"/>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="7">
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="B20" s="1">
-        <f t="shared" si="12"/>
+      <c r="C20" s="1">
+        <f t="shared" si="13"/>
         <v>84.48</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1">
+      <c r="D20" s="1"/>
+      <c r="E20" s="1">
+        <f t="shared" si="14"/>
+        <v>84.100000000000023</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1">
+        <f t="shared" si="15"/>
+        <v>72.939999999999984</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1">
+        <f t="shared" si="16"/>
+        <v>76.019999999999982</v>
+      </c>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="7">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="C21" s="1">
         <f t="shared" si="13"/>
-        <v>84.100000000000023</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1">
+        <v>84.84</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1">
         <f t="shared" si="14"/>
-        <v>72.939999999999984</v>
-      </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1">
+        <v>84.500000000000028</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1">
         <f t="shared" si="15"/>
-        <v>76.019999999999982</v>
-      </c>
-      <c r="I20" s="8"/>
-    </row>
-    <row r="21" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7">
-        <f t="shared" si="0"/>
-        <v>95</v>
-      </c>
-      <c r="B21" s="1">
-        <f t="shared" si="12"/>
-        <v>84.84</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1">
-        <f t="shared" si="13"/>
-        <v>84.500000000000028</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1">
-        <f t="shared" si="14"/>
         <v>74.119999999999976</v>
       </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1">
-        <f t="shared" si="15"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1">
+        <f t="shared" si="16"/>
         <v>78.559999999999974</v>
       </c>
-      <c r="I21" s="8"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="7">
-        <f t="shared" si="0"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B22" s="7">
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="B22" s="1">
+      <c r="C22" s="1">
         <v>85.2</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1">
         <v>84.9</v>
       </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1">
+      <c r="F22" s="1"/>
+      <c r="G22" s="1">
         <v>75.3</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1">
+      <c r="H22" s="1"/>
+      <c r="I22" s="1">
         <v>81.099999999999994</v>
       </c>
-      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>